<commit_message>
update for new version ICS from MBP
</commit_message>
<xml_diff>
--- a/checktool_v1.0/Template_213.xlsx
+++ b/checktool_v1.0/Template_213.xlsx
@@ -204,9 +204,6 @@
     <t>Zero Amount Authorized is supported</t>
   </si>
   <si>
-    <t>Check Box95</t>
-  </si>
-  <si>
     <t>Variable Transaction Amount is supported</t>
   </si>
   <si>
@@ -365,6 +362,9 @@
   </si>
   <si>
     <t>MSD Zero Amount Authorized is supported</t>
+  </si>
+  <si>
+    <t>Check Box95</t>
   </si>
   <si>
     <t>6. General Reader Options</t>
@@ -642,10 +642,10 @@
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="0.0"/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -709,11 +709,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -740,15 +739,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -756,7 +765,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -771,38 +780,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -816,6 +824,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -823,21 +838,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -860,7 +860,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -872,7 +890,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -884,121 +1028,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1010,37 +1040,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1059,41 +1059,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1137,6 +1102,41 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1154,145 +1154,145 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1776,8 +1776,8 @@
   </sheetPr>
   <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
@@ -2173,7 +2173,7 @@
         <v>60</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="21"/>
@@ -2188,10 +2188,10 @@
         <v>3.15</v>
       </c>
       <c r="D23" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="22" t="s">
         <v>62</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>63</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="21"/>
@@ -2206,10 +2206,10 @@
         <v>3.16</v>
       </c>
       <c r="D24" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="22" t="s">
         <v>64</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>65</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="21"/>
@@ -2224,10 +2224,10 @@
         <v>3.17</v>
       </c>
       <c r="D25" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="22" t="s">
         <v>66</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>67</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="21"/>
@@ -2242,10 +2242,10 @@
         <v>3.19</v>
       </c>
       <c r="D26" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="22" t="s">
         <v>68</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>69</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="21"/>
@@ -2260,10 +2260,10 @@
         <v>3.2</v>
       </c>
       <c r="D27" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="22" t="s">
         <v>70</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>71</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="21"/>
@@ -2278,10 +2278,10 @@
         <v>3.21</v>
       </c>
       <c r="D28" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="22" t="s">
         <v>72</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>73</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="21"/>
@@ -2296,10 +2296,10 @@
         <v>3.22</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="22" t="s">
         <v>74</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>75</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="21"/>
@@ -2311,16 +2311,16 @@
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="E30" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="F30" s="17" t="s">
         <v>77</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>78</v>
       </c>
       <c r="G30" s="21"/>
     </row>
@@ -2334,10 +2334,10 @@
         <v>3.23</v>
       </c>
       <c r="D31" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="22" t="s">
         <v>79</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>80</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="21"/>
@@ -2352,7 +2352,7 @@
         <v>3.25</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E32" s="22" t="s">
         <v>53</v>
@@ -2370,10 +2370,10 @@
         <v>3.26</v>
       </c>
       <c r="D33" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" s="22" t="s">
         <v>82</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>83</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="21"/>
@@ -2388,10 +2388,10 @@
         <v>3.27</v>
       </c>
       <c r="D34" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" s="22" t="s">
         <v>84</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>85</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="21"/>
@@ -2406,10 +2406,10 @@
         <v>3.28</v>
       </c>
       <c r="D35" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" s="22" t="s">
         <v>86</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>87</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="21"/>
@@ -2424,10 +2424,10 @@
         <v>3.29</v>
       </c>
       <c r="D36" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" s="22" t="s">
         <v>88</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>89</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="21"/>
@@ -2435,7 +2435,7 @@
     <row r="37" ht="28" spans="1:7">
       <c r="A37" s="9"/>
       <c r="B37" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="13"/>
@@ -2453,10 +2453,10 @@
         <v>4.1</v>
       </c>
       <c r="D38" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E38" s="22" t="s">
         <v>91</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>92</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="21"/>
@@ -2468,13 +2468,13 @@
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="E39" s="22" t="s">
         <v>94</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>95</v>
       </c>
       <c r="F39" s="14"/>
       <c r="G39" s="21"/>
@@ -2486,13 +2486,13 @@
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D40" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="E40" s="22" t="s">
         <v>97</v>
-      </c>
-      <c r="E40" s="22" t="s">
-        <v>98</v>
       </c>
       <c r="F40" s="14"/>
       <c r="G40" s="21"/>
@@ -2507,10 +2507,10 @@
         <v>4.2</v>
       </c>
       <c r="D41" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E41" s="22" t="s">
         <v>99</v>
-      </c>
-      <c r="E41" s="22" t="s">
-        <v>100</v>
       </c>
       <c r="F41" s="14"/>
       <c r="G41" s="21"/>
@@ -2522,13 +2522,13 @@
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="D42" s="17" t="s">
+      <c r="E42" s="22" t="s">
         <v>102</v>
-      </c>
-      <c r="E42" s="22" t="s">
-        <v>103</v>
       </c>
       <c r="F42" s="14"/>
       <c r="G42" s="21"/>
@@ -2540,20 +2540,20 @@
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D43" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="D43" s="17" t="s">
+      <c r="E43" s="22" t="s">
         <v>105</v>
-      </c>
-      <c r="E43" s="22" t="s">
-        <v>106</v>
       </c>
       <c r="F43" s="14"/>
       <c r="G43" s="21"/>
     </row>
     <row r="44" spans="2:7">
       <c r="B44" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="13"/>
@@ -2571,10 +2571,10 @@
         <v>5.1</v>
       </c>
       <c r="D45" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E45" s="22" t="s">
         <v>108</v>
-      </c>
-      <c r="E45" s="22" t="s">
-        <v>109</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="21"/>
@@ -2589,10 +2589,10 @@
         <v>5.2</v>
       </c>
       <c r="D46" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E46" s="22" t="s">
         <v>110</v>
-      </c>
-      <c r="E46" s="22" t="s">
-        <v>111</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="21"/>
@@ -2607,10 +2607,10 @@
         <v>5.3</v>
       </c>
       <c r="D47" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E47" s="22" t="s">
         <v>112</v>
-      </c>
-      <c r="E47" s="22" t="s">
-        <v>113</v>
       </c>
       <c r="F47" s="7"/>
       <c r="G47" s="21"/>
@@ -2625,10 +2625,10 @@
         <v>5.7</v>
       </c>
       <c r="D48" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E48" s="22" t="s">
         <v>114</v>
-      </c>
-      <c r="E48" s="22" t="s">
-        <v>61</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="21"/>

</xml_diff>